<commit_message>
days_per_month ipynb in helper dir; csv in data_output dir
</commit_message>
<xml_diff>
--- a/data_output/results_of_grouping_attempts_rus_holidays.xlsx
+++ b/data_output/results_of_grouping_attempts_rus_holidays.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgaid\Google Drive\Colab Notebooks\NRUHSE_2_Kaggle_Coursera\final\Kag\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2324A44-BC2E-4E17-B982-42E87704E0A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8F9570-1793-4CA2-B04D-964E243DF066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8E922349-5CAB-4486-B52B-DE742A6FBB1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E922349-5CAB-4486-B52B-DE742A6FBB1B}"/>
   </bookViews>
   <sheets>
     <sheet name="item_category_id" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="347">
   <si>
     <t>n_nodes</t>
   </si>
@@ -1117,6 +1117,42 @@
   </si>
   <si>
     <t>Same with shop 20 and shop 9</t>
+  </si>
+  <si>
+    <t>jan</t>
+  </si>
+  <si>
+    <t>feb</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>apr</t>
+  </si>
+  <si>
+    <t>may</t>
+  </si>
+  <si>
+    <t>june</t>
+  </si>
+  <si>
+    <t>july</t>
+  </si>
+  <si>
+    <t>aug</t>
+  </si>
+  <si>
+    <t>sept</t>
+  </si>
+  <si>
+    <t>oct</t>
+  </si>
+  <si>
+    <t>nov</t>
+  </si>
+  <si>
+    <t>dec</t>
   </si>
 </sst>
 </file>
@@ -1305,6 +1341,99 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>324868</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>10442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B02F351-CDA2-4A26-90B3-9F93084D1FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10382250" y="18392775"/>
+          <a:ext cx="7297168" cy="6573167"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>343913</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>57929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DCF674E-DDDC-421F-A1AA-86EBAA8CE074}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10439400" y="11239500"/>
+          <a:ext cx="7259063" cy="5582429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -7450,8 +7579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0140B458-2DC9-48A0-9DAB-116645715FDE}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8877,7 +9006,7 @@
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="18">
         <v>44187</v>
       </c>
@@ -8891,28 +9020,49 @@
         <v>246</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>291</v>
       </c>
       <c r="C117" s="11" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>2013</v>
+      </c>
+      <c r="H117" t="s">
+        <v>335</v>
+      </c>
+      <c r="I117">
+        <v>6</v>
+      </c>
+      <c r="J117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>267</v>
       </c>
       <c r="D118" s="11" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H118" t="s">
+        <v>336</v>
+      </c>
+      <c r="I118">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>271</v>
       </c>
@@ -8923,8 +9073,17 @@
       <c r="D119" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H119" t="s">
+        <v>337</v>
+      </c>
+      <c r="I119">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="18">
         <v>43831</v>
       </c>
@@ -8937,8 +9096,14 @@
       <c r="D120" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H120" t="s">
+        <v>338</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="18">
         <v>43832</v>
       </c>
@@ -8951,8 +9116,14 @@
       <c r="D121" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H121" t="s">
+        <v>339</v>
+      </c>
+      <c r="I121">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="18">
         <v>43833</v>
       </c>
@@ -8965,8 +9136,14 @@
       <c r="D122" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H122" t="s">
+        <v>340</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="18">
         <v>43834</v>
       </c>
@@ -8979,8 +9156,14 @@
       <c r="D123" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H123" t="s">
+        <v>341</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="18">
         <v>43837</v>
       </c>
@@ -8993,8 +9176,14 @@
       <c r="D124" s="2" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H124" t="s">
+        <v>342</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="18">
         <v>43838</v>
       </c>
@@ -9007,8 +9196,14 @@
       <c r="D125" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H125" t="s">
+        <v>343</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="18">
         <v>43844</v>
       </c>
@@ -9021,8 +9216,14 @@
       <c r="D126" s="2" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H126" t="s">
+        <v>344</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="18">
         <v>43854</v>
       </c>
@@ -9035,12 +9236,24 @@
       <c r="D127" s="2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H127" t="s">
+        <v>345</v>
+      </c>
+      <c r="I127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
+      <c r="H128" t="s">
+        <v>346</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="18">
@@ -9495,6 +9708,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId36"/>
+  <drawing r:id="rId37"/>
 </worksheet>
 </file>
 
@@ -9502,7 +9716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526057EE-278E-4C29-AEF5-9C7139A14A53}">
   <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v9 split, cleaned a bit, improved NLP
</commit_message>
<xml_diff>
--- a/data_output/results_of_grouping_attempts_rus_holidays.xlsx
+++ b/data_output/results_of_grouping_attempts_rus_holidays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgaid\Google Drive\Colab Notebooks\NRUHSE_2_Kaggle_Coursera\final\Kag\data_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8F9570-1793-4CA2-B04D-964E243DF066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ED65A0-B3B2-4682-9507-F54B4EF14E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8E922349-5CAB-4486-B52B-DE742A6FBB1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8E922349-5CAB-4486-B52B-DE742A6FBB1B}"/>
   </bookViews>
   <sheets>
     <sheet name="item_category_id" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="shop_id" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="367">
   <si>
     <t>n_nodes</t>
   </si>
@@ -1154,12 +1155,72 @@
   <si>
     <t>dec</t>
   </si>
+  <si>
+    <t>done: Thu 18:47:36 06/11/20</t>
+  </si>
+  <si>
+    <t>Correlation Threshold (1000x): 880</t>
+  </si>
+  <si>
+    <t>Fill fillna(0) before computing correlations?: True</t>
+  </si>
+  <si>
+    <t>Grouping time period: by item_id</t>
+  </si>
+  <si>
+    <t>Grouping category: by shop_id</t>
+  </si>
+  <si>
+    <t>Aggregation column: sum of sales within a item_id for each shop_id</t>
+  </si>
+  <si>
+    <t>Total number of ids in all suggested clusters): 34</t>
+  </si>
+  <si>
+    <t>Number of *unique* ids contained in all clusters: 34</t>
+  </si>
+  <si>
+    <t>In the following table, "w" refers to the weights between graph nodes = 1000x correlation coefficient:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   n_nodes  w_avg  w_sum  w_max  w_min  w_std                                                                                     cluster_members  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0        2    920    920    920    920      0                                                                                            [57, 58]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1        3    899   2697    907    887  8.641                                                                                        [21, 25, 42]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2        3    899   2698    905    888  8.014                                                                                        [28, 31, 54]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3       26    895  69836    929    881 10.354  [2, 3, 4, 5, 6, 7, 10, 14, 15, 16, 18, 19, 24, 26, 27, 35, 37, 38, 41, 45, 46, 47, 50, 52, 53, 59]   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                 category_names  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                             [Yakutsk Ordzhonikidze, 56, Yakutsk TC "Central"]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                             [Moscow MTRTS "Afi Mall", Moscow SEC "Atrium", St. Petersburg TK "Nevsky Center"]  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                            [Moscow shopping center "MEGA Teply Stan" II of, Moscow shopping center "Semyonov", Khimki shopping center "Mega"]  </t>
+  </si>
+  <si>
+    <t>3  [Adygea TC "Mega", Balashikha TRC "October-Kinomir", Volzhsky mall "Volga Mall", Vologda SEC "Marmalade", Voronezh (Plekhanovskaya, 13), Voronezh SEC "Maksimir", Zhukovsky Street. Chkalov 39m?, Kazan shopping mall of "Parkhouse" II of, Kaluga SEC "XXI Century", Kolomna shopping center "Rio", Krasnoyarsk SC "June", Kursk TC "Pushkin", Moscow TK "Budenovsky" (pav.K7), Moscow shopping mall "area" (Belyaevo), Moscow shopping center "MEGA Belaya Dacha II", Nizhny Novgorod SEC "Fantasy", Novosibirsk shopping center "Mega", Omsk TC "Mega", RostovNaDonu TC "Mega", Samara mall of "Parkhouse", Sergiev Posad TC "7Ya", Surgut SEC "City Mall", Tyumen SC "Goodwin", Ufa TC "Central", Ufa TC "Family" 2, Yaroslavl shopping center "Altair"]</t>
+  </si>
+  <si>
+    <t>by day</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1237,6 +1298,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1286,7 +1353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1322,6 +1389,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1490,7 +1558,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>249556</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>86295</xdr:rowOff>
+      <xdr:rowOff>92010</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1532,7 +1600,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>278135</xdr:colOff>
+      <xdr:colOff>285755</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>76769</xdr:rowOff>
     </xdr:to>
@@ -1578,7 +1646,7 @@
       <xdr:col>22</xdr:col>
       <xdr:colOff>230504</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>181532</xdr:rowOff>
+      <xdr:rowOff>170102</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1620,9 +1688,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>278135</xdr:colOff>
+      <xdr:colOff>285755</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>162479</xdr:rowOff>
+      <xdr:rowOff>168194</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1664,9 +1732,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>316241</xdr:colOff>
+      <xdr:colOff>323861</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>29111</xdr:rowOff>
+      <xdr:rowOff>17681</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1708,7 +1776,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>163819</xdr:colOff>
+      <xdr:colOff>169534</xdr:colOff>
       <xdr:row>121</xdr:row>
       <xdr:rowOff>558</xdr:rowOff>
     </xdr:to>
@@ -2049,64 +2117,64 @@
       <selection activeCell="I462" sqref="I462"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="32.42578125" customWidth="1"/>
-    <col min="9" max="9" width="163.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="32.44140625" customWidth="1"/>
+    <col min="9" max="9" width="163.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -2135,7 +2203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -2164,7 +2232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -2193,7 +2261,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2</v>
       </c>
@@ -2222,7 +2290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>3</v>
       </c>
@@ -2251,7 +2319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>4</v>
       </c>
@@ -2280,7 +2348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -2309,7 +2377,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -2338,7 +2406,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>7</v>
       </c>
@@ -2367,68 +2435,68 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -2457,7 +2525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2486,7 +2554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2515,7 +2583,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -2544,7 +2612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2573,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -2602,7 +2670,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2631,12 +2699,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2653,7 +2721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -2670,7 +2738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1</v>
       </c>
@@ -2687,7 +2755,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -2704,7 +2772,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>3</v>
       </c>
@@ -2721,7 +2789,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4</v>
       </c>
@@ -2738,7 +2806,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>5</v>
       </c>
@@ -2755,7 +2823,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>6</v>
       </c>
@@ -2772,7 +2840,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>7</v>
       </c>
@@ -2789,7 +2857,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>8</v>
       </c>
@@ -2806,7 +2874,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>9</v>
       </c>
@@ -2823,68 +2891,68 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>47</v>
       </c>
@@ -2913,7 +2981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -2942,7 +3010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -2971,7 +3039,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2</v>
       </c>
@@ -3000,7 +3068,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>3</v>
       </c>
@@ -3029,7 +3097,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -3058,7 +3126,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>5</v>
       </c>
@@ -3087,7 +3155,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>6</v>
       </c>
@@ -3116,7 +3184,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>7</v>
       </c>
@@ -3145,7 +3213,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8</v>
       </c>
@@ -3174,68 +3242,68 @@
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="92" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>0</v>
       </c>
@@ -3261,7 +3329,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>0</v>
       </c>
@@ -3290,7 +3358,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1</v>
       </c>
@@ -3319,7 +3387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>2</v>
       </c>
@@ -3348,7 +3416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>3</v>
       </c>
@@ -3377,7 +3445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>4</v>
       </c>
@@ -3406,7 +3474,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>5</v>
       </c>
@@ -3435,7 +3503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>6</v>
       </c>
@@ -3464,7 +3532,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>7</v>
       </c>
@@ -3493,12 +3561,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>49</v>
       </c>
@@ -3512,7 +3580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>0</v>
       </c>
@@ -3532,7 +3600,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>1</v>
       </c>
@@ -3549,7 +3617,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>2</v>
       </c>
@@ -3566,7 +3634,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>3</v>
       </c>
@@ -3583,7 +3651,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>4</v>
       </c>
@@ -3600,7 +3668,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>5</v>
       </c>
@@ -3617,7 +3685,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>6</v>
       </c>
@@ -3634,7 +3702,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>7</v>
       </c>
@@ -3651,7 +3719,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>8</v>
       </c>
@@ -3668,7 +3736,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>9</v>
       </c>
@@ -3685,68 +3753,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="126" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>0</v>
       </c>
@@ -3772,7 +3840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>0</v>
       </c>
@@ -3801,12 +3869,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>49</v>
       </c>
@@ -3820,7 +3888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>0</v>
       </c>
@@ -3837,7 +3905,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>1</v>
       </c>
@@ -3854,7 +3922,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>2</v>
       </c>
@@ -3871,7 +3939,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>3</v>
       </c>
@@ -3888,7 +3956,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>4</v>
       </c>
@@ -3905,7 +3973,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>5</v>
       </c>
@@ -3922,7 +3990,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>6</v>
       </c>
@@ -3939,7 +4007,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>7</v>
       </c>
@@ -3956,7 +4024,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>8</v>
       </c>
@@ -3973,7 +4041,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>9</v>
       </c>
@@ -3990,68 +4058,68 @@
         <v>53</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>0</v>
       </c>
@@ -4077,7 +4145,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>0</v>
       </c>
@@ -4106,7 +4174,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>1</v>
       </c>
@@ -4135,7 +4203,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>2</v>
       </c>
@@ -4164,68 +4232,68 @@
         <v>126</v>
       </c>
     </row>
-    <row r="179" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
         <v>0</v>
       </c>
@@ -4251,7 +4319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>0</v>
       </c>
@@ -4280,7 +4348,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>1</v>
       </c>
@@ -4309,7 +4377,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>2</v>
       </c>
@@ -4338,12 +4406,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B201" t="s">
         <v>49</v>
       </c>
@@ -4357,7 +4425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>0</v>
       </c>
@@ -4374,7 +4442,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>1</v>
       </c>
@@ -4391,7 +4459,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>2</v>
       </c>
@@ -4408,7 +4476,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>3</v>
       </c>
@@ -4425,7 +4493,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>4</v>
       </c>
@@ -4442,7 +4510,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>5</v>
       </c>
@@ -4459,7 +4527,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>6</v>
       </c>
@@ -4476,7 +4544,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>7</v>
       </c>
@@ -4493,7 +4561,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>8</v>
       </c>
@@ -4510,7 +4578,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>9</v>
       </c>
@@ -4527,68 +4595,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="213" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B230" t="s">
         <v>0</v>
       </c>
@@ -4614,7 +4682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>0</v>
       </c>
@@ -4643,7 +4711,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>1</v>
       </c>
@@ -4672,12 +4740,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B235" t="s">
         <v>49</v>
       </c>
@@ -4691,7 +4759,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>0</v>
       </c>
@@ -4708,7 +4776,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>1</v>
       </c>
@@ -4725,7 +4793,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>2</v>
       </c>
@@ -4742,7 +4810,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>3</v>
       </c>
@@ -4759,7 +4827,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>4</v>
       </c>
@@ -4776,7 +4844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>5</v>
       </c>
@@ -4793,7 +4861,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>6</v>
       </c>
@@ -4810,7 +4878,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>7</v>
       </c>
@@ -4827,7 +4895,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>8</v>
       </c>
@@ -4844,7 +4912,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>9</v>
       </c>
@@ -4861,68 +4929,68 @@
         <v>140</v>
       </c>
     </row>
-    <row r="247" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B263" t="s">
         <v>0</v>
       </c>
@@ -4948,7 +5016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>0</v>
       </c>
@@ -4977,7 +5045,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>1</v>
       </c>
@@ -5006,7 +5074,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>2</v>
       </c>
@@ -5035,7 +5103,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>3</v>
       </c>
@@ -5064,12 +5132,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B270" t="s">
         <v>49</v>
       </c>
@@ -5083,7 +5151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>0</v>
       </c>
@@ -5100,7 +5168,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>1</v>
       </c>
@@ -5117,7 +5185,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>2</v>
       </c>
@@ -5134,7 +5202,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>3</v>
       </c>
@@ -5151,7 +5219,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>4</v>
       </c>
@@ -5168,7 +5236,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>5</v>
       </c>
@@ -5185,7 +5253,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>6</v>
       </c>
@@ -5202,7 +5270,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>7</v>
       </c>
@@ -5219,7 +5287,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>8</v>
       </c>
@@ -5236,7 +5304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>9</v>
       </c>
@@ -5253,73 +5321,73 @@
         <v>55</v>
       </c>
     </row>
-    <row r="282" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="285" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A285" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B298" t="s">
         <v>0</v>
       </c>
@@ -5345,7 +5413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>0</v>
       </c>
@@ -5374,7 +5442,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>1</v>
       </c>
@@ -5403,7 +5471,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>2</v>
       </c>
@@ -5432,7 +5500,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>3</v>
       </c>
@@ -5461,12 +5529,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B306" t="s">
         <v>49</v>
       </c>
@@ -5480,7 +5548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>0</v>
       </c>
@@ -5497,7 +5565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>1</v>
       </c>
@@ -5514,7 +5582,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>2</v>
       </c>
@@ -5531,7 +5599,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>3</v>
       </c>
@@ -5548,7 +5616,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>4</v>
       </c>
@@ -5565,7 +5633,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>5</v>
       </c>
@@ -5582,7 +5650,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>6</v>
       </c>
@@ -5599,7 +5667,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>7</v>
       </c>
@@ -5616,7 +5684,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>8</v>
       </c>
@@ -5633,7 +5701,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>9</v>
       </c>
@@ -5650,23 +5718,23 @@
         <v>159</v>
       </c>
     </row>
-    <row r="318" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A321" s="8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A322" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A323" s="8" t="s">
         <v>139</v>
       </c>
@@ -5674,52 +5742,52 @@
         <v>176</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A324" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A327" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B334" t="s">
         <v>0</v>
       </c>
@@ -5745,7 +5813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>0</v>
       </c>
@@ -5774,7 +5842,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>1</v>
       </c>
@@ -5803,7 +5871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>2</v>
       </c>
@@ -5832,7 +5900,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>3</v>
       </c>
@@ -5861,7 +5929,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>4</v>
       </c>
@@ -5890,12 +5958,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B342" t="s">
         <v>49</v>
       </c>
@@ -5909,7 +5977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>0</v>
       </c>
@@ -5926,7 +5994,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>1</v>
       </c>
@@ -5943,7 +6011,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>2</v>
       </c>
@@ -5960,7 +6028,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>3</v>
       </c>
@@ -5977,7 +6045,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>4</v>
       </c>
@@ -5994,7 +6062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>5</v>
       </c>
@@ -6011,7 +6079,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>6</v>
       </c>
@@ -6028,7 +6096,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>7</v>
       </c>
@@ -6045,7 +6113,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>8</v>
       </c>
@@ -6062,7 +6130,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>9</v>
       </c>
@@ -6079,73 +6147,73 @@
         <v>168</v>
       </c>
     </row>
-    <row r="354" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A363" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B370" t="s">
         <v>0</v>
       </c>
@@ -6171,7 +6239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A371">
         <v>0</v>
       </c>
@@ -6200,7 +6268,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A372">
         <v>1</v>
       </c>
@@ -6229,7 +6297,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A373">
         <v>2</v>
       </c>
@@ -6258,7 +6326,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A374">
         <v>3</v>
       </c>
@@ -6287,12 +6355,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B377" t="s">
         <v>49</v>
       </c>
@@ -6306,7 +6374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A378">
         <v>0</v>
       </c>
@@ -6323,7 +6391,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A379">
         <v>1</v>
       </c>
@@ -6340,7 +6408,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A380">
         <v>2</v>
       </c>
@@ -6357,7 +6425,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A381">
         <v>3</v>
       </c>
@@ -6374,7 +6442,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A382">
         <v>4</v>
       </c>
@@ -6391,7 +6459,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A383">
         <v>5</v>
       </c>
@@ -6408,7 +6476,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A384">
         <v>6</v>
       </c>
@@ -6425,7 +6493,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A385">
         <v>7</v>
       </c>
@@ -6442,7 +6510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A386">
         <v>8</v>
       </c>
@@ -6459,7 +6527,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A387">
         <v>9</v>
       </c>
@@ -6476,13 +6544,13 @@
         <v>165</v>
       </c>
     </row>
-    <row r="389" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="391" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>174</v>
       </c>
@@ -6490,7 +6558,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A393" s="8" t="s">
         <v>63</v>
       </c>
@@ -6498,7 +6566,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>139</v>
       </c>
@@ -6506,52 +6574,52 @@
         <v>187</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B405" t="s">
         <v>0</v>
       </c>
@@ -6577,7 +6645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A406">
         <v>0</v>
       </c>
@@ -6606,7 +6674,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A407">
         <v>1</v>
       </c>
@@ -6635,7 +6703,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A408">
         <v>2</v>
       </c>
@@ -6664,7 +6732,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A409">
         <v>3</v>
       </c>
@@ -6693,7 +6761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A410">
         <v>4</v>
       </c>
@@ -6722,7 +6790,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A411">
         <v>5</v>
       </c>
@@ -6751,7 +6819,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A412">
         <v>6</v>
       </c>
@@ -6780,7 +6848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A413">
         <v>7</v>
       </c>
@@ -6809,12 +6877,12 @@
         <v>106</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B416" t="s">
         <v>49</v>
       </c>
@@ -6828,7 +6896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A417">
         <v>0</v>
       </c>
@@ -6845,7 +6913,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A418">
         <v>1</v>
       </c>
@@ -6862,7 +6930,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A419">
         <v>2</v>
       </c>
@@ -6879,7 +6947,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A420">
         <v>3</v>
       </c>
@@ -6896,7 +6964,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A421">
         <v>4</v>
       </c>
@@ -6913,7 +6981,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A422">
         <v>5</v>
       </c>
@@ -6930,7 +6998,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423">
         <v>6</v>
       </c>
@@ -6947,7 +7015,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A424">
         <v>7</v>
       </c>
@@ -6964,7 +7032,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A425">
         <v>8</v>
       </c>
@@ -6981,7 +7049,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A426">
         <v>9</v>
       </c>
@@ -6998,73 +7066,73 @@
         <v>165</v>
       </c>
     </row>
-    <row r="429" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="433" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="434" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="435" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="436" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="437" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="438" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A438" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="439" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="440" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="441" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="442" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="443" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="445" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B445" t="s">
         <v>0</v>
       </c>
@@ -7090,7 +7158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="446" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A446">
         <v>0</v>
       </c>
@@ -7119,7 +7187,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="447" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A447">
         <v>1</v>
       </c>
@@ -7148,7 +7216,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="448" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A448">
         <v>2</v>
       </c>
@@ -7177,7 +7245,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A449">
         <v>3</v>
       </c>
@@ -7206,7 +7274,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A450">
         <v>4</v>
       </c>
@@ -7235,7 +7303,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A451">
         <v>5</v>
       </c>
@@ -7264,7 +7332,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="452" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A452">
         <v>6</v>
       </c>
@@ -7293,7 +7361,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A453">
         <v>7</v>
       </c>
@@ -7322,7 +7390,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A454">
         <v>8</v>
       </c>
@@ -7351,7 +7419,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A455">
         <v>9</v>
       </c>
@@ -7380,12 +7448,12 @@
         <v>214</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B458" t="s">
         <v>49</v>
       </c>
@@ -7399,7 +7467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A459">
         <v>0</v>
       </c>
@@ -7416,7 +7484,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="460" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A460">
         <v>1</v>
       </c>
@@ -7433,7 +7501,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="461" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A461">
         <v>2</v>
       </c>
@@ -7450,7 +7518,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="462" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A462">
         <v>3</v>
       </c>
@@ -7467,7 +7535,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A463">
         <v>4</v>
       </c>
@@ -7484,7 +7552,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="464" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A464">
         <v>5</v>
       </c>
@@ -7501,7 +7569,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="465" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A465">
         <v>6</v>
       </c>
@@ -7518,7 +7586,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="466" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A466">
         <v>7</v>
       </c>
@@ -7535,7 +7603,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="467" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A467">
         <v>8</v>
       </c>
@@ -7552,7 +7620,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="468" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A468">
         <v>9</v>
       </c>
@@ -7579,35 +7647,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0140B458-2DC9-48A0-9DAB-116645715FDE}">
   <dimension ref="A1:Q163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>223</v>
       </c>
@@ -7618,7 +7686,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>267</v>
       </c>
@@ -7626,7 +7694,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43831</v>
       </c>
@@ -7643,7 +7711,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43832</v>
       </c>
@@ -7660,7 +7728,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43833</v>
       </c>
@@ -7677,7 +7745,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43833</v>
       </c>
@@ -7694,7 +7762,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43834</v>
       </c>
@@ -7711,7 +7779,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43835</v>
       </c>
@@ -7728,7 +7796,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43836</v>
       </c>
@@ -7742,7 +7810,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43837</v>
       </c>
@@ -7759,7 +7827,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43838</v>
       </c>
@@ -7773,7 +7841,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43839</v>
       </c>
@@ -7799,7 +7867,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43844</v>
       </c>
@@ -7825,7 +7893,7 @@
         <v>43946</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -7843,7 +7911,7 @@
         <v>44115</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43875</v>
       </c>
@@ -7869,7 +7937,7 @@
         <v>44115</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43884</v>
       </c>
@@ -7895,7 +7963,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43888</v>
       </c>
@@ -7921,13 +7989,13 @@
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43898</v>
       </c>
@@ -7941,7 +8009,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43899</v>
       </c>
@@ -7961,7 +8029,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43911</v>
       </c>
@@ -7981,13 +8049,13 @@
         <v>317</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43933</v>
       </c>
@@ -8004,7 +8072,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -8013,7 +8081,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43952</v>
       </c>
@@ -8027,7 +8095,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43955</v>
       </c>
@@ -8044,7 +8112,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43960</v>
       </c>
@@ -8061,7 +8129,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43962</v>
       </c>
@@ -8075,7 +8143,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43967</v>
       </c>
@@ -8092,13 +8160,13 @@
         <v>322</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
       <c r="D34" s="16"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43994</v>
       </c>
@@ -8112,7 +8180,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>44000</v>
       </c>
@@ -8126,7 +8194,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>44003</v>
       </c>
@@ -8140,13 +8208,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>44025</v>
       </c>
@@ -8160,7 +8228,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>44030</v>
       </c>
@@ -8177,13 +8245,13 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>44075</v>
       </c>
@@ -8197,7 +8265,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>44097</v>
       </c>
@@ -8211,7 +8279,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>44098</v>
       </c>
@@ -8228,13 +8296,13 @@
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
       <c r="D45" s="16"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>44119</v>
       </c>
@@ -8248,13 +8316,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>44139</v>
       </c>
@@ -8268,13 +8336,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="16"/>
       <c r="D49" s="16"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>44187</v>
       </c>
@@ -8288,7 +8356,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>44189</v>
       </c>
@@ -8302,12 +8370,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>284</v>
       </c>
@@ -8315,7 +8383,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>267</v>
       </c>
@@ -8323,7 +8391,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>271</v>
       </c>
@@ -8335,7 +8403,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="18">
         <v>43831</v>
       </c>
@@ -8349,7 +8417,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="18">
         <v>43832</v>
       </c>
@@ -8363,7 +8431,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="18">
         <v>43833</v>
       </c>
@@ -8377,7 +8445,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="18">
         <v>43834</v>
       </c>
@@ -8391,7 +8459,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="18">
         <v>43835</v>
       </c>
@@ -8405,7 +8473,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="18">
         <v>43836</v>
       </c>
@@ -8419,7 +8487,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="18">
         <v>43837</v>
       </c>
@@ -8433,7 +8501,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="18">
         <v>43838</v>
       </c>
@@ -8447,7 +8515,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="18">
         <v>43844</v>
       </c>
@@ -8461,7 +8529,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="18">
         <v>43844</v>
       </c>
@@ -8475,13 +8543,13 @@
         <v>239</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="18">
         <v>43875</v>
       </c>
@@ -8495,7 +8563,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="18">
         <v>43883</v>
       </c>
@@ -8509,7 +8577,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="18">
         <v>43884</v>
       </c>
@@ -8523,13 +8591,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="18">
         <v>43898</v>
       </c>
@@ -8543,7 +8611,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="18">
         <v>43899</v>
       </c>
@@ -8557,7 +8625,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="18">
         <v>43900</v>
       </c>
@@ -8571,7 +8639,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="18">
         <v>43910</v>
       </c>
@@ -8585,13 +8653,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="18">
         <v>43941</v>
       </c>
@@ -8608,13 +8676,13 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="18">
         <v>43952</v>
       </c>
@@ -8628,7 +8696,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="18">
         <v>43953</v>
       </c>
@@ -8642,7 +8710,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="18">
         <v>43954</v>
       </c>
@@ -8656,7 +8724,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="18">
         <v>43955</v>
       </c>
@@ -8670,7 +8738,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="18">
         <v>43960</v>
       </c>
@@ -8684,7 +8752,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="18">
         <v>43961</v>
       </c>
@@ -8698,7 +8766,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="18">
         <v>43962</v>
       </c>
@@ -8712,7 +8780,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="18">
         <v>43978</v>
       </c>
@@ -8726,13 +8794,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="18">
         <v>43989</v>
       </c>
@@ -8746,7 +8814,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="18">
         <v>43994</v>
       </c>
@@ -8760,7 +8828,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="18">
         <v>43995</v>
       </c>
@@ -8774,7 +8842,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="18">
         <v>43996</v>
       </c>
@@ -8788,7 +8856,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="18">
         <v>43997</v>
       </c>
@@ -8802,7 +8870,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="18">
         <v>44003</v>
       </c>
@@ -8816,7 +8884,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="18">
         <v>44011</v>
       </c>
@@ -8830,13 +8898,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="18">
         <v>44036</v>
       </c>
@@ -8850,7 +8918,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="18">
         <v>44041</v>
       </c>
@@ -8864,19 +8932,19 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="18">
         <v>44075</v>
       </c>
@@ -8890,7 +8958,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="18">
         <v>44097</v>
       </c>
@@ -8904,13 +8972,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="18">
         <v>44108</v>
       </c>
@@ -8924,7 +8992,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="18">
         <v>44129</v>
       </c>
@@ -8938,13 +9006,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="18">
         <v>44136</v>
       </c>
@@ -8958,7 +9026,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="18">
         <v>44137</v>
       </c>
@@ -8972,7 +9040,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="18">
         <v>44138</v>
       </c>
@@ -8986,7 +9054,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="18">
         <v>44139</v>
       </c>
@@ -9000,13 +9068,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="18">
         <v>44187</v>
       </c>
@@ -9020,12 +9088,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="11" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>291</v>
       </c>
@@ -9045,7 +9113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>267</v>
       </c>
@@ -9062,7 +9130,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>271</v>
       </c>
@@ -9083,7 +9151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="18">
         <v>43831</v>
       </c>
@@ -9103,7 +9171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="18">
         <v>43832</v>
       </c>
@@ -9123,7 +9191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="18">
         <v>43833</v>
       </c>
@@ -9143,7 +9211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="18">
         <v>43834</v>
       </c>
@@ -9163,7 +9231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="18">
         <v>43837</v>
       </c>
@@ -9183,7 +9251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="18">
         <v>43838</v>
       </c>
@@ -9203,7 +9271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" s="18">
         <v>43844</v>
       </c>
@@ -9223,7 +9291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" s="18">
         <v>43854</v>
       </c>
@@ -9243,7 +9311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -9255,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="18">
         <v>43875</v>
       </c>
@@ -9269,7 +9337,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="18">
         <v>43884</v>
       </c>
@@ -9283,13 +9351,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="18">
         <v>43898</v>
       </c>
@@ -9303,7 +9371,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="18">
         <v>43910</v>
       </c>
@@ -9317,19 +9385,19 @@
         <v>246</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="18">
         <v>43952</v>
       </c>
@@ -9343,7 +9411,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="18">
         <v>43953</v>
       </c>
@@ -9357,7 +9425,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="18">
         <v>43954</v>
       </c>
@@ -9371,7 +9439,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="18">
         <v>43956</v>
       </c>
@@ -9388,7 +9456,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="18">
         <v>43960</v>
       </c>
@@ -9402,7 +9470,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="18">
         <v>43961</v>
       </c>
@@ -9416,7 +9484,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="18">
         <v>43961</v>
       </c>
@@ -9430,13 +9498,13 @@
         <v>226</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="18">
         <v>43988</v>
       </c>
@@ -9450,7 +9518,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="18">
         <v>43994</v>
       </c>
@@ -9464,7 +9532,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="18">
         <v>44003</v>
       </c>
@@ -9478,13 +9546,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="18">
         <v>44021</v>
       </c>
@@ -9498,13 +9566,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="18">
         <v>44046</v>
       </c>
@@ -9518,7 +9586,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="18">
         <v>44051</v>
       </c>
@@ -9532,13 +9600,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="18">
         <v>44075</v>
       </c>
@@ -9552,7 +9620,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="18">
         <v>44097</v>
       </c>
@@ -9566,13 +9634,13 @@
         <v>246</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="18">
         <v>44119</v>
       </c>
@@ -9586,13 +9654,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="18">
         <v>44139</v>
       </c>
@@ -9606,7 +9674,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="18">
         <v>44140</v>
       </c>
@@ -9620,13 +9688,13 @@
         <v>231</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="18">
         <v>44186</v>
       </c>
@@ -9640,7 +9708,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="18">
         <v>44195</v>
       </c>
@@ -9654,7 +9722,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="18">
         <v>44196</v>
       </c>
@@ -9714,20 +9782,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526057EE-278E-4C29-AEF5-9C7139A14A53}">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -9735,7 +9803,10 @@
         <v>325</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="Z5" s="19"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>326</v>
       </c>
@@ -9743,7 +9814,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>329</v>
       </c>
@@ -9751,12 +9822,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>330</v>
       </c>
@@ -9764,18 +9835,132 @@
         <v>333</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>334</v>
       </c>
     </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>350</v>
+      </c>
+      <c r="E182" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>365</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>